<commit_message>
Changed charts to plot relative to mission success and whether or not the spacecraft system started conjoined
</commit_message>
<xml_diff>
--- a/CMQA/Mission Configuration Trade Study/RCL-0-CMQA1 Rascal Mission Configuration Trade Study Martix.xlsx
+++ b/CMQA/Mission Configuration Trade Study/RCL-0-CMQA1 Rascal Mission Configuration Trade Study Martix.xlsx
@@ -4,19 +4,23 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="20115" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="20115" windowHeight="8505" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="1" r:id="rId1"/>
-    <sheet name="Data" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="All Mission Data" sheetId="2" r:id="rId2"/>
+    <sheet name="Launched Mission Data" sheetId="3" r:id="rId3"/>
+    <sheet name="All Missions Graph" sheetId="6" r:id="rId4"/>
+    <sheet name="Launched Mission Graph" sheetId="7" r:id="rId5"/>
+    <sheet name="Cost Comparison" sheetId="8" r:id="rId6"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="125725" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="93">
   <si>
     <t>Document Title</t>
   </si>
@@ -246,27 +250,6 @@
     <t>Weight</t>
   </si>
   <si>
-    <t>2900 lbs</t>
-  </si>
-  <si>
-    <t>220 lbs</t>
-  </si>
-  <si>
-    <t>18 lbs</t>
-  </si>
-  <si>
-    <t>790 lbs</t>
-  </si>
-  <si>
-    <t>36 lbs</t>
-  </si>
-  <si>
-    <t>40 lbs</t>
-  </si>
-  <si>
-    <t>62 lbs</t>
-  </si>
-  <si>
     <t>AFRL/Boeing</t>
   </si>
   <si>
@@ -288,9 +271,6 @@
     <t>Two spacecraft performed inspections of each other and third passive spacecraft</t>
   </si>
   <si>
-    <t>1000 lbs</t>
-  </si>
-  <si>
     <t>ProxOps-1</t>
   </si>
   <si>
@@ -298,6 +278,27 @@
   </si>
   <si>
     <t>One spacecraft will be released from the other while the other circumnaviages and captures images of it</t>
+  </si>
+  <si>
+    <t>Rascal</t>
+  </si>
+  <si>
+    <t>Saint Louis University</t>
+  </si>
+  <si>
+    <t>Maybe</t>
+  </si>
+  <si>
+    <t>You know</t>
+  </si>
+  <si>
+    <t>IDK</t>
+  </si>
+  <si>
+    <t>Separable?</t>
+  </si>
+  <si>
+    <t>Cost (million dollars)</t>
   </si>
 </sst>
 </file>
@@ -444,6 +445,3443 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Conjoined</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('All Mission Data'!$F$5,'All Mission Data'!$F$10,'All Mission Data'!$F$14,'All Mission Data'!$F$13,'All Mission Data'!$F$8)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('All Mission Data'!$E$5,'All Mission Data'!$E$8,'All Mission Data'!$E$13,'All Mission Data'!$E$14,'All Mission Data'!$E$10)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2900</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Separated</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('All Mission Data'!$F$2,'All Mission Data'!$F$3,'All Mission Data'!$F$4,'All Mission Data'!$F$6,'All Mission Data'!$F$7,'All Mission Data'!$F$9,'All Mission Data'!$F$11,'All Mission Data'!$F$12)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('All Mission Data'!$E$2,'All Mission Data'!$E$3,'All Mission Data'!$E$4,'All Mission Data'!$E$6,'All Mission Data'!$E$7,'All Mission Data'!$E$9,'All Mission Data'!$E$11,'All Mission Data'!$E$12)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>790</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="142555776"/>
+        <c:axId val="142664064"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="142555776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="4"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>Number of Spacecraft</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="142664064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="142664064"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1">
+                    <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>Weight</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" b="1" baseline="0">
+                    <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t> (lbs)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" b="1">
+                  <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="142555776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.87309439052791449"/>
+          <c:y val="0.46978108559436549"/>
+          <c:w val="8.4426734725136426E-2"/>
+          <c:h val="6.8515499109389144E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr>
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:userShapes r:id="rId1"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Succeeded</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Launched Mission Data'!$D$2,'Launched Mission Data'!$D$10,'Launched Mission Data'!$D$11,'Launched Mission Data'!$D$12)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Launched Mission Data'!$F$2,'Launched Mission Data'!$F$10,'Launched Mission Data'!$F$11,'Launched Mission Data'!$F$12)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2900</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Failed</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Launched Mission Data'!$D$4,'Launched Mission Data'!$D$6)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Launched Mission Data'!$F$4,'Launched Mission Data'!$F$6)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>790</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Rascal</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Launched Mission Data'!$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Launched Mission Data'!$F$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="144570624"/>
+        <c:axId val="144802176"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="144570624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="4"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>Number of Spacecraft</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="144802176"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="144802176"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1">
+                    <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>Weight</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" b="1" baseline="0">
+                    <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t> (lbs)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" b="1">
+                  <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="144570624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.87735692589045322"/>
+          <c:y val="0.42639970284349893"/>
+          <c:w val="8.6023354500107951E-2"/>
+          <c:h val="0.10277324866408372"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr>
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:userShapes r:id="rId1"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Succeeded</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Launched Mission Data'!$D$2,'Launched Mission Data'!$D$10,'Launched Mission Data'!$D$11,'Launched Mission Data'!$D$12)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Launched Mission Data'!$H$2,'Launched Mission Data'!$H$10,'Launched Mission Data'!$H$11,'Launched Mission Data'!$H$12)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Failed</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Launched Mission Data'!$D$4,'Launched Mission Data'!$D$6)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Launched Mission Data'!$H$4,'Launched Mission Data'!$H$6)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Rascal</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Launched Mission Data'!$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Launched Mission Data'!$H$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="144833920"/>
+        <c:axId val="143853056"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="144833920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="4"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>Number of Spacecraft</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="143853056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="143853056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1">
+                    <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>Cost </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" b="1" baseline="0">
+                    <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>(lMillions of Dollars)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" b="1">
+                  <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="144833920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.88907223738528507"/>
+          <c:y val="0.42704973268953667"/>
+          <c:w val="8.6023354500107951E-2"/>
+          <c:h val="0.10277324866408372"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr>
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:userShapes r:id="rId1"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="78" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="78" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="78" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8670192" cy="6288942"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.31268</cdr:x>
+      <cdr:y>0.65437</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.41897</cdr:x>
+      <cdr:y>0.69709</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2710960" y="4115289"/>
+          <a:ext cx="921547" cy="268654"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>SNAP-1</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.31408</cdr:x>
+      <cdr:y>0.61359</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.42037</cdr:x>
+      <cdr:y>0.65631</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2723172" y="3858847"/>
+          <a:ext cx="921547" cy="268654"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>GLADOS</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.31268</cdr:x>
+      <cdr:y>0.48932</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.41897</cdr:x>
+      <cdr:y>0.53204</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2710960" y="3077308"/>
+          <a:ext cx="921547" cy="268654"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>XSS-10</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.31268</cdr:x>
+      <cdr:y>0.36699</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.41897</cdr:x>
+      <cdr:y>0.40971</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="5" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2710961" y="2307981"/>
+          <a:ext cx="921547" cy="268654"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>XSS-11</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.31268</cdr:x>
+      <cdr:y>0.2466</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.41897</cdr:x>
+      <cdr:y>0.28932</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="6" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2710960" y="1550865"/>
+          <a:ext cx="921547" cy="268654"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>DART</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.53944</cdr:x>
+      <cdr:y>0.55534</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.64573</cdr:x>
+      <cdr:y>0.59806</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="7" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="4677018" y="3492499"/>
+          <a:ext cx="921547" cy="268654"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Rascal</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.53803</cdr:x>
+      <cdr:y>0.60777</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.64432</cdr:x>
+      <cdr:y>0.65049</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="8" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="4664807" y="3822210"/>
+          <a:ext cx="921547" cy="268654"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>PONSFD</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.53662</cdr:x>
+      <cdr:y>0.4466</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.64291</cdr:x>
+      <cdr:y>0.48932</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="9" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="4652595" y="2808654"/>
+          <a:ext cx="921547" cy="268654"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>MSAT</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.53944</cdr:x>
+      <cdr:y>0.12233</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.69437</cdr:x>
+      <cdr:y>0.17087</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="10" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="4677018" y="769327"/>
+          <a:ext cx="1343269" cy="305288"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Orbital</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> Express</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.76338</cdr:x>
+      <cdr:y>0.2233</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.86967</cdr:x>
+      <cdr:y>0.26602</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="11" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="6618653" y="1404326"/>
+          <a:ext cx="921547" cy="268654"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>MiTEx</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.53521</cdr:x>
+      <cdr:y>0.58058</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.66492</cdr:x>
+      <cdr:y>0.61942</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="12" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="4640385" y="3651252"/>
+          <a:ext cx="1124595" cy="244230"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>STRaND-2</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8670192" cy="6288942"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.31268</cdr:x>
+      <cdr:y>0.48932</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.39577</cdr:x>
+      <cdr:y>0.53204</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2710961" y="3077308"/>
+          <a:ext cx="720482" cy="268654"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>XSS-10</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.31268</cdr:x>
+      <cdr:y>0.36699</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.39577</cdr:x>
+      <cdr:y>0.40971</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="5" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2710962" y="2307981"/>
+          <a:ext cx="720482" cy="268654"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>XSS-11</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.31268</cdr:x>
+      <cdr:y>0.2466</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.39577</cdr:x>
+      <cdr:y>0.28932</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="6" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2710961" y="1550865"/>
+          <a:ext cx="720482" cy="268654"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>DART</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.53944</cdr:x>
+      <cdr:y>0.55534</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.62254</cdr:x>
+      <cdr:y>0.59806</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="7" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="4677019" y="3492499"/>
+          <a:ext cx="720482" cy="268654"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Rascal</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.53944</cdr:x>
+      <cdr:y>0.12233</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.69155</cdr:x>
+      <cdr:y>0.17087</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="10" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="4677047" y="769326"/>
+          <a:ext cx="1318817" cy="305266"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Orbital</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> Express</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.76338</cdr:x>
+      <cdr:y>0.2233</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.84648</cdr:x>
+      <cdr:y>0.26602</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="11" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="6618654" y="1404326"/>
+          <a:ext cx="720482" cy="268654"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>MiTEx</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.32113</cdr:x>
+      <cdr:y>0.60971</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.40422</cdr:x>
+      <cdr:y>0.65243</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="13" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2784231" y="3834423"/>
+          <a:ext cx="720406" cy="268664"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>SNAP-1</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8670192" cy="6288942"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.30564</cdr:x>
+      <cdr:y>0.63107</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.38873</cdr:x>
+      <cdr:y>0.67379</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2649938" y="3968748"/>
+          <a:ext cx="720406" cy="268664"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>XSS-10</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.30564</cdr:x>
+      <cdr:y>0.68932</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.38873</cdr:x>
+      <cdr:y>0.73204</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="5" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2649939" y="4335095"/>
+          <a:ext cx="720406" cy="268663"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>XSS-11</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.30564</cdr:x>
+      <cdr:y>0.65825</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.38873</cdr:x>
+      <cdr:y>0.70097</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="6" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2649939" y="4139699"/>
+          <a:ext cx="720406" cy="268664"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>DART</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.53662</cdr:x>
+      <cdr:y>0.87379</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.61972</cdr:x>
+      <cdr:y>0.91651</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="7" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="4652625" y="5495193"/>
+          <a:ext cx="720493" cy="268664"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Rascal</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.5324</cdr:x>
+      <cdr:y>0.12816</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.68592</cdr:x>
+      <cdr:y>0.1767</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="10" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="4615991" y="805961"/>
+          <a:ext cx="1331028" cy="305266"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Orbital</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> Express</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.7662</cdr:x>
+      <cdr:y>0.80971</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.8493</cdr:x>
+      <cdr:y>0.85243</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="11" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="6643074" y="5092206"/>
+          <a:ext cx="720493" cy="268663"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>MiTEx</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.30564</cdr:x>
+      <cdr:y>0.8699</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.38873</cdr:x>
+      <cdr:y>0.91262</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="13" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2649931" y="5470776"/>
+          <a:ext cx="720406" cy="268663"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>SNAP-1</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -873,22 +4311,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="41.85546875" customWidth="1"/>
     <col min="10" max="10" width="19.5703125" customWidth="1"/>
     <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="37.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -946,8 +4385,8 @@
       <c r="D2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>77</v>
+      <c r="E2" s="7">
+        <v>220</v>
       </c>
       <c r="F2" s="7">
         <v>1</v>
@@ -985,8 +4424,8 @@
       <c r="D3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>78</v>
+      <c r="E3" s="7">
+        <v>18</v>
       </c>
       <c r="F3" s="7">
         <v>1</v>
@@ -1024,8 +4463,8 @@
       <c r="D4" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>79</v>
+      <c r="E4" s="7">
+        <v>790</v>
       </c>
       <c r="F4" s="7">
         <v>1</v>
@@ -1063,8 +4502,8 @@
       <c r="D5" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>19</v>
+      <c r="E5" s="7">
+        <v>100</v>
       </c>
       <c r="F5" s="7">
         <v>2</v>
@@ -1102,8 +4541,8 @@
       <c r="D6" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>78</v>
+      <c r="E6" s="7">
+        <v>18</v>
       </c>
       <c r="F6" s="7">
         <v>1</v>
@@ -1143,8 +4582,8 @@
       <c r="D7" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>80</v>
+      <c r="E7" s="7">
+        <v>26</v>
       </c>
       <c r="F7" s="7">
         <v>2</v>
@@ -1184,8 +4623,8 @@
       <c r="D8" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>81</v>
+      <c r="E8" s="7">
+        <v>22</v>
       </c>
       <c r="F8" s="7">
         <v>2</v>
@@ -1225,8 +4664,8 @@
       <c r="D9" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>19</v>
+      <c r="E9" s="7">
+        <v>11</v>
       </c>
       <c r="F9" s="7">
         <v>1</v>
@@ -1266,8 +4705,8 @@
       <c r="D10" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>76</v>
+      <c r="E10" s="7">
+        <v>2900</v>
       </c>
       <c r="F10" s="7">
         <v>2</v>
@@ -1279,7 +4718,7 @@
         <v>69</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="J10" s="10" t="s">
         <v>73</v>
@@ -1299,7 +4738,7 @@
         <v>74</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C11" s="9">
         <v>37622</v>
@@ -1307,8 +4746,8 @@
       <c r="D11" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>82</v>
+      <c r="E11" s="7">
+        <v>62</v>
       </c>
       <c r="F11" s="7">
         <v>1</v>
@@ -1317,7 +4756,7 @@
         <v>19</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="I11" s="10" t="s">
         <v>19</v>
@@ -1337,10 +4776,10 @@
     </row>
     <row r="12" spans="1:13" ht="30">
       <c r="A12" s="7" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C12" s="9">
         <v>38869</v>
@@ -1348,8 +4787,8 @@
       <c r="D12" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>90</v>
+      <c r="E12" s="7">
+        <v>1000</v>
       </c>
       <c r="F12" s="7">
         <v>3</v>
@@ -1358,7 +4797,7 @@
         <v>38</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="I12" s="10" t="s">
         <v>19</v>
@@ -1367,7 +4806,7 @@
         <v>21</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="L12" s="7" t="s">
         <v>23</v>
@@ -1378,10 +4817,10 @@
     </row>
     <row r="13" spans="1:13" ht="45">
       <c r="A13" s="7" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>19</v>
@@ -1389,8 +4828,8 @@
       <c r="D13" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="7" t="s">
-        <v>19</v>
+      <c r="E13" s="7">
+        <v>100</v>
       </c>
       <c r="F13" s="7">
         <v>2</v>
@@ -1399,7 +4838,7 @@
         <v>23</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="I13" s="10" t="s">
         <v>19</v>
@@ -1418,19 +4857,45 @@
       </c>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
+      <c r="A14" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="7">
+        <v>30</v>
+      </c>
+      <c r="F14" s="7">
+        <v>2</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="L14" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="M14" s="7" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="7"/>
@@ -1469,6 +4934,359 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" activeCellId="7" sqref="D2 D10 D11 D12 H12 H11 H10 H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="9">
+        <v>38443</v>
+      </c>
+      <c r="D2" s="7">
+        <v>1</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="7">
+        <v>220</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="9">
+        <v>38443</v>
+      </c>
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="7">
+        <v>790</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="7">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" spans="1:8" ht="30">
+      <c r="A6" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="9">
+        <v>36678</v>
+      </c>
+      <c r="D6" s="7">
+        <v>1</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="7">
+        <v>18</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="7">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="9">
+        <v>39142</v>
+      </c>
+      <c r="D10" s="7">
+        <v>2</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="7">
+        <v>2900</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="7">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="9">
+        <v>37622</v>
+      </c>
+      <c r="D11" s="7">
+        <v>1</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="7">
+        <v>62</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="9">
+        <v>38869</v>
+      </c>
+      <c r="D12" s="7">
+        <v>3</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="7">
+        <v>2</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="7">
+        <v>30</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="H14" s="7">
+        <v>0.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Changed previous mission chart sto that it plots weight vs cost. Also added aerocube 4 and DRAGONsat to plot
</commit_message>
<xml_diff>
--- a/CMQA/Mission Configuration Trade Study/RCL-0-CMQA1 Rascal Mission Configuration Trade Study Martix.xlsx
+++ b/CMQA/Mission Configuration Trade Study/RCL-0-CMQA1 Rascal Mission Configuration Trade Study Martix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="20115" windowHeight="8505" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="20115" windowHeight="8505" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="103">
   <si>
     <t>Document Title</t>
   </si>
@@ -299,6 +299,36 @@
   </si>
   <si>
     <t>Cost (million dollars)</t>
+  </si>
+  <si>
+    <t>Aerocube 4</t>
+  </si>
+  <si>
+    <t>Aerosapce Corperation</t>
+  </si>
+  <si>
+    <t>Stationkeeping by altering ballistic coefficient</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>GPS, Motion Processors</t>
+  </si>
+  <si>
+    <t>$200 Thousand</t>
+  </si>
+  <si>
+    <t>Weight (kg)</t>
+  </si>
+  <si>
+    <t>Aerospace Corperation</t>
+  </si>
+  <si>
+    <t>DRAGONsat</t>
+  </si>
+  <si>
+    <t>University of Texas Austin</t>
   </si>
 </sst>
 </file>
@@ -407,21 +437,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -436,6 +454,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -593,11 +638,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="142555776"/>
-        <c:axId val="142664064"/>
+        <c:axId val="83244160"/>
+        <c:axId val="83246080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="142555776"/>
+        <c:axId val="83244160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -626,13 +671,13 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142664064"/>
+        <c:crossAx val="83246080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="142664064"/>
+        <c:axId val="83246080"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -672,7 +717,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142555776"/>
+        <c:crossAx val="83244160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -683,8 +728,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.87309439052791449"/>
-          <c:y val="0.46978108559436549"/>
+          <c:x val="0.8730943905279146"/>
+          <c:y val="0.46978108559436554"/>
           <c:w val="8.4426734725136426E-2"/>
           <c:h val="6.8515499109389144E-2"/>
         </c:manualLayout>
@@ -857,11 +902,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="144570624"/>
-        <c:axId val="144802176"/>
+        <c:axId val="93535232"/>
+        <c:axId val="93550464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="144570624"/>
+        <c:axId val="93535232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -890,13 +935,13 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144802176"/>
+        <c:crossAx val="93550464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="144802176"/>
+        <c:axId val="93550464"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -936,7 +981,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144570624"/>
+        <c:crossAx val="93535232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -947,10 +992,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.87735692589045322"/>
-          <c:y val="0.42639970284349893"/>
-          <c:w val="8.6023354500107951E-2"/>
-          <c:h val="0.10277324866408372"/>
+          <c:x val="0.87735692589045311"/>
+          <c:y val="0.42639970284349898"/>
+          <c:w val="8.6023354500107965E-2"/>
+          <c:h val="0.10277324866408373"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -1002,31 +1047,37 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>('Launched Mission Data'!$D$2,'Launched Mission Data'!$D$10,'Launched Mission Data'!$D$11,'Launched Mission Data'!$D$12)</c:f>
+              <c:f>('Launched Mission Data'!$G$2,'Launched Mission Data'!$G$10,'Launched Mission Data'!$G$11,'Launched Mission Data'!$G$12,'Launched Mission Data'!$G$15,'Launched Mission Data'!$G$16)</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>99.790239999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1315.4168</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28.122703999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>453.59199999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>7.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>('Launched Mission Data'!$H$2,'Launched Mission Data'!$H$10,'Launched Mission Data'!$H$11,'Launched Mission Data'!$H$12)</c:f>
+              <c:f>('Launched Mission Data'!$I$2,'Launched Mission Data'!$I$10,'Launched Mission Data'!$I$11,'Launched Mission Data'!$I$12,'Launched Mission Data'!$I$15,'Launched Mission Data'!$I$16)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>80</c:v>
                 </c:pt>
@@ -1038,6 +1089,12 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1056,22 +1113,22 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>('Launched Mission Data'!$D$4,'Launched Mission Data'!$D$6)</c:f>
+              <c:f>('Launched Mission Data'!$G$4,'Launched Mission Data'!$G$6)</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>8.1646560000000008</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>('Launched Mission Data'!$H$4,'Launched Mission Data'!$H$6)</c:f>
+              <c:f>('Launched Mission Data'!$I$4,'Launched Mission Data'!$I$6)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1096,21 +1153,28 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:marker>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Launched Mission Data'!$D$14</c:f>
+              <c:f>'Launched Mission Data'!$G$14</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>13.607759999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Launched Mission Data'!$H$14</c:f>
+              <c:f>'Launched Mission Data'!$I$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1121,14 +1185,14 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="144833920"/>
-        <c:axId val="143853056"/>
+        <c:axId val="93589504"/>
+        <c:axId val="93591424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="144833920"/>
+        <c:axId val="93589504"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
-          <c:max val="4"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:title>
@@ -1145,22 +1209,21 @@
                     <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
                     <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
                   </a:rPr>
-                  <a:t>Number of Spacecraft</a:t>
+                  <a:t>Weight (kg)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
           <c:layout/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143853056"/>
+        <c:crossAx val="93591424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="143853056"/>
+        <c:axId val="93591424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1199,7 +1262,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144833920"/>
+        <c:crossAx val="93589504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1210,10 +1273,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.88907223738528507"/>
-          <c:y val="0.42704973268953667"/>
-          <c:w val="8.6023354500107951E-2"/>
-          <c:h val="0.10277324866408372"/>
+          <c:x val="8.3438405977630026E-2"/>
+          <c:y val="2.3166217783531798E-2"/>
+          <c:w val="8.6023354500107965E-2"/>
+          <c:h val="0.10277324866408373"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -1270,7 +1333,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="78" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="78" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3176,12 +3239,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.30564</cdr:x>
-      <cdr:y>0.63107</cdr:y>
+      <cdr:x>0.40987</cdr:x>
+      <cdr:y>0.63495</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.38873</cdr:x>
-      <cdr:y>0.67379</cdr:y>
+      <cdr:x>0.49296</cdr:x>
+      <cdr:y>0.67767</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -3190,12 +3253,23 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="2649938" y="3968748"/>
-          <a:ext cx="720406" cy="268664"/>
+          <a:off x="3553611" y="3993186"/>
+          <a:ext cx="720407" cy="268663"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
       </cdr:spPr>
       <cdr:txBody>
         <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
@@ -3265,8 +3339,12 @@
           </a:lvl9pPr>
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1100">
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
               <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
               <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
             </a:rPr>
@@ -3278,12 +3356,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.30564</cdr:x>
-      <cdr:y>0.68932</cdr:y>
+      <cdr:x>0.53099</cdr:x>
+      <cdr:y>0.68349</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.38873</cdr:x>
-      <cdr:y>0.73204</cdr:y>
+      <cdr:x>0.61408</cdr:x>
+      <cdr:y>0.72621</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -3292,12 +3370,23 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="2649939" y="4335095"/>
-          <a:ext cx="720406" cy="268663"/>
+          <a:off x="4603802" y="4298459"/>
+          <a:ext cx="720407" cy="268664"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
       </cdr:spPr>
       <cdr:txBody>
         <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
@@ -3367,8 +3456,12 @@
           </a:lvl9pPr>
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1100">
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
               <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
               <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
             </a:rPr>
@@ -3380,12 +3473,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.30564</cdr:x>
-      <cdr:y>0.65825</cdr:y>
+      <cdr:x>0.5324</cdr:x>
+      <cdr:y>0.63495</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.38873</cdr:x>
-      <cdr:y>0.70097</cdr:y>
+      <cdr:x>0.61549</cdr:x>
+      <cdr:y>0.67767</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -3394,12 +3487,23 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="2649939" y="4139699"/>
-          <a:ext cx="720406" cy="268664"/>
+          <a:off x="4616014" y="3993158"/>
+          <a:ext cx="720407" cy="268664"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
       </cdr:spPr>
       <cdr:txBody>
         <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
@@ -3469,8 +3573,12 @@
           </a:lvl9pPr>
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1100">
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
               <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
               <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
             </a:rPr>
@@ -3482,12 +3590,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.53662</cdr:x>
-      <cdr:y>0.87379</cdr:y>
+      <cdr:x>0.33662</cdr:x>
+      <cdr:y>0.8602</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.61972</cdr:x>
-      <cdr:y>0.91651</cdr:y>
+      <cdr:x>0.41972</cdr:x>
+      <cdr:y>0.90292</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -3496,12 +3604,20 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="4652625" y="5495193"/>
-          <a:ext cx="720493" cy="268664"/>
+          <a:off x="2918561" y="5409733"/>
+          <a:ext cx="720493" cy="268663"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:srgbClr val="00B050"/>
+        </a:solidFill>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
       </cdr:spPr>
       <cdr:txBody>
         <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
@@ -3553,8 +3669,9 @@
           </a:lvl9pPr>
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1100">
+            <a:rPr lang="en-US" sz="1100" b="1">
               <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
               <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
             </a:rPr>
@@ -3566,12 +3683,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.5324</cdr:x>
-      <cdr:y>0.12816</cdr:y>
+      <cdr:x>0.78733</cdr:x>
+      <cdr:y>0.12622</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.68592</cdr:x>
-      <cdr:y>0.1767</cdr:y>
+      <cdr:x>0.93803</cdr:x>
+      <cdr:y>0.17476</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -3580,12 +3697,22 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="4615991" y="805961"/>
-          <a:ext cx="1331028" cy="305266"/>
+          <a:off x="6826299" y="793780"/>
+          <a:ext cx="1306586" cy="305265"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:schemeClr val="bg2">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
       </cdr:spPr>
       <cdr:txBody>
         <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
@@ -3655,21 +3782,31 @@
           </a:lvl9pPr>
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1100">
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
               <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
               <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
             </a:rPr>
             <a:t>Orbital</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
               <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
               <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
             </a:rPr>
             <a:t> Express</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1100">
+          <a:endParaRPr lang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
             <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
             <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
           </a:endParaRPr>
@@ -3679,11 +3816,11 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.7662</cdr:x>
+      <cdr:x>0.67888</cdr:x>
       <cdr:y>0.80971</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.8493</cdr:x>
+      <cdr:x>0.76198</cdr:x>
       <cdr:y>0.85243</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
@@ -3693,12 +3830,22 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="6643074" y="5092206"/>
-          <a:ext cx="720493" cy="268663"/>
+          <a:off x="5885986" y="5092219"/>
+          <a:ext cx="720493" cy="268664"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:schemeClr val="bg2">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
       </cdr:spPr>
       <cdr:txBody>
         <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
@@ -3768,8 +3915,12 @@
           </a:lvl9pPr>
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1100">
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
               <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
               <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
             </a:rPr>
@@ -3781,12 +3932,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.30564</cdr:x>
-      <cdr:y>0.8699</cdr:y>
+      <cdr:x>0.30987</cdr:x>
+      <cdr:y>0.76893</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.38873</cdr:x>
-      <cdr:y>0.91262</cdr:y>
+      <cdr:x>0.39296</cdr:x>
+      <cdr:y>0.81165</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -3795,12 +3946,23 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="2649931" y="5470776"/>
-          <a:ext cx="720406" cy="268663"/>
+          <a:off x="2686592" y="4835752"/>
+          <a:ext cx="720407" cy="268663"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:schemeClr val="tx1">
+            <a:lumMod val="95000"/>
+            <a:lumOff val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
       </cdr:spPr>
       <cdr:txBody>
         <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
@@ -3870,13 +4032,1340 @@
           </a:lvl9pPr>
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1100">
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
               <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
               <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
             </a:rPr>
             <a:t>SNAP-1</a:t>
           </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.1507</cdr:x>
+      <cdr:y>0.72039</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.26901</cdr:x>
+      <cdr:y>0.76505</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="9" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1306634" y="4530480"/>
+          <a:ext cx="1025769" cy="280866"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:schemeClr val="tx1">
+            <a:lumMod val="95000"/>
+            <a:lumOff val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>DRAGONSat</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.07606</cdr:x>
+      <cdr:y>0.80388</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.19155</cdr:x>
+      <cdr:y>0.85049</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="12" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="659423" y="5055577"/>
+          <a:ext cx="1001346" cy="293077"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:schemeClr val="tx1">
+            <a:lumMod val="95000"/>
+            <a:lumOff val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Aerocube-4</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.08732</cdr:x>
+      <cdr:y>0.85049</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.1338</cdr:x>
+      <cdr:y>0.89515</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="15" name="Straight Arrow Connector 14"/>
+        <cdr:cNvSpPr/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1">
+          <a:off x="757114" y="5348654"/>
+          <a:ext cx="402981" cy="280865"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="38100">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.20845</cdr:x>
+      <cdr:y>0.76505</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.2662</cdr:x>
+      <cdr:y>0.8932</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="16" name="Straight Arrow Connector 15"/>
+        <cdr:cNvSpPr/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1807309" y="4811346"/>
+          <a:ext cx="500672" cy="805962"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="38100">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.28732</cdr:x>
+      <cdr:y>0.80971</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.34507</cdr:x>
+      <cdr:y>0.89903</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="17" name="Straight Arrow Connector 16"/>
+        <cdr:cNvSpPr/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1">
+          <a:off x="2491154" y="5092213"/>
+          <a:ext cx="500673" cy="561730"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="38100">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.07887</cdr:x>
+      <cdr:y>0.61748</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.35211</cdr:x>
+      <cdr:y>0.67184</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="19" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="683847" y="3883268"/>
+          <a:ext cx="2369038" cy="341924"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:schemeClr val="tx1">
+            <a:lumMod val="95000"/>
+            <a:lumOff val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>CubeSat Missions: 1-15 kg</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.22817</cdr:x>
+      <cdr:y>0.5068</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.52254</cdr:x>
+      <cdr:y>0.56117</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="21" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1978270" y="3187211"/>
+          <a:ext cx="2552211" cy="341924"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> Microsat</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Missions: 10-100 kg</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.37183</cdr:x>
+      <cdr:y>0.21553</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.67606</cdr:x>
+      <cdr:y>0.2699</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="23" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3223847" y="1355480"/>
+          <a:ext cx="2637692" cy="341924"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:schemeClr val="bg2">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Military</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Missions: &gt;100</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> kg</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.00986</cdr:x>
+      <cdr:y>0.69903</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.45775</cdr:x>
+      <cdr:y>0.99029</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="24" name="Oval 23"/>
+        <cdr:cNvSpPr/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="85481" y="4396154"/>
+          <a:ext cx="3883269" cy="1831731"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </cdr:style>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.38451</cdr:x>
+      <cdr:y>0.56893</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.63099</cdr:x>
+      <cdr:y>0.78835</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="25" name="Oval 24"/>
+        <cdr:cNvSpPr/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3333750" y="3577981"/>
+          <a:ext cx="2137019" cy="1379904"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </cdr:style>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.64689</cdr:x>
+      <cdr:y>0.00089</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.95053</cdr:x>
+      <cdr:y>0.95525</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="26" name="Oval 25"/>
+        <cdr:cNvSpPr/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="16944572">
+          <a:off x="3924030" y="1690234"/>
+          <a:ext cx="6001892" cy="2632625"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:solidFill>
+            <a:schemeClr val="bg2">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </cdr:style>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </cdr:txBody>
     </cdr:sp>
@@ -4185,113 +5674,113 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="9">
         <v>41608</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -4311,8 +5800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView topLeftCell="D1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4326,606 +5815,632 @@
     <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="41.85546875" customWidth="1"/>
     <col min="10" max="10" width="19.5703125" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="37.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="30">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="5">
         <v>38443</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="3">
         <v>220</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="3">
         <v>1</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10" t="s">
+      <c r="I2" s="6"/>
+      <c r="J2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="30">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="3">
         <v>18</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="3">
         <v>1</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10" t="s">
+      <c r="I3" s="6"/>
+      <c r="J3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="M3" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="30">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="5">
         <v>38443</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="3">
         <v>790</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="3">
         <v>1</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10" t="s">
+      <c r="I4" s="6"/>
+      <c r="J4" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="K4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="L4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="M4" s="7" t="s">
+      <c r="M4" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="30">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="3">
         <v>100</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="3">
         <v>2</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10" t="s">
+      <c r="I5" s="6"/>
+      <c r="J5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="K5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="L5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M5" s="7" t="s">
+      <c r="M5" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="30">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="5">
         <v>36678</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="3">
         <v>18</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="3">
         <v>1</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="I6" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="J6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="K6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="L6" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="M6" s="8" t="s">
+      <c r="M6" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="45">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="3">
         <v>26</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="3">
         <v>2</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="J7" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="K7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="L7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M7" s="7" t="s">
+      <c r="M7" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="30">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="3">
         <v>22</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="3">
         <v>2</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="I8" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="J8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="K8" s="7" t="s">
+      <c r="K8" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L8" s="7" t="s">
+      <c r="L8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="7" t="s">
+      <c r="M8" s="3" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="30">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="3">
         <v>11</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="3">
         <v>1</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H9" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="I9" s="10" t="s">
+      <c r="I9" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="10" t="s">
+      <c r="J9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K9" s="7" t="s">
+      <c r="K9" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="L9" s="7" t="s">
+      <c r="L9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M9" s="7" t="s">
+      <c r="M9" s="3" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="45">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="5">
         <v>39142</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="3">
         <v>2900</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="3">
         <v>2</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="H10" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="I10" s="10" t="s">
+      <c r="I10" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="J10" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="K10" s="7" t="s">
+      <c r="K10" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="L10" s="7" t="s">
+      <c r="L10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="M10" s="7" t="s">
+      <c r="M10" s="3" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="30">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="5">
         <v>37622</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="3">
         <v>62</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="3">
         <v>1</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="I11" s="10" t="s">
+      <c r="I11" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="10" t="s">
+      <c r="J11" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="K11" s="7" t="s">
+      <c r="K11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L11" s="7" t="s">
+      <c r="L11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="M11" s="7" t="s">
+      <c r="M11" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="30">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="5">
         <v>38869</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="3">
         <v>1000</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="3">
         <v>3</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H12" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="I12" s="10" t="s">
+      <c r="I12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J12" s="10" t="s">
+      <c r="J12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K12" s="7" t="s">
+      <c r="K12" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="L12" s="7" t="s">
+      <c r="L12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="M12" s="7" t="s">
+      <c r="M12" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="45">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="3">
         <v>100</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="3">
         <v>2</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="H13" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="I13" s="10" t="s">
+      <c r="I13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="10" t="s">
+      <c r="J13" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K13" s="7" t="s">
+      <c r="K13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L13" s="7" t="s">
+      <c r="L13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M13" s="7" t="s">
+      <c r="M13" s="3" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="3">
         <v>30</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="3">
         <v>2</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G14" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="H14" s="10" t="s">
+      <c r="H14" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="I14" s="10" t="s">
+      <c r="I14" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="J14" s="10" t="s">
+      <c r="J14" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="K14" s="7" t="s">
+      <c r="K14" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="L14" s="7" t="s">
+      <c r="L14" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="M14" s="7" t="s">
+      <c r="M14" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
+    <row r="15" spans="1:13" ht="30">
+      <c r="A15" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" s="5">
+        <v>41153</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1</v>
+      </c>
+      <c r="F15" s="3">
+        <v>3</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4934,350 +6449,461 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" activeCellId="7" sqref="D2 D10 D11 D12 H12 H11 H10 H2"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.140625" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:9">
+      <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="5">
         <v>38443</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="3">
         <v>1</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="3">
         <v>220</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="11">
+        <f>F2*0.453592</f>
+        <v>99.790239999999997</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="7">
+      <c r="I2" s="3">
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:9">
+      <c r="A3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7" t="s">
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7" t="s">
+      <c r="F3" s="3"/>
+      <c r="G3" s="11">
+        <f t="shared" ref="G3:G15" si="0">F3*0.453592</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="7"/>
+      <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:9">
+      <c r="A4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="5">
         <v>38443</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="3">
         <v>1</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="3">
         <v>790</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="11">
+        <v>98</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H4" s="7">
+      <c r="I4" s="3">
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:9">
+      <c r="A5" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7" t="s">
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7" t="s">
+      <c r="F5" s="3"/>
+      <c r="G5" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="7"/>
+      <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:8" ht="30">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:9" ht="30">
+      <c r="A6" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="5">
         <v>36678</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="3">
         <v>1</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="3">
         <v>18</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="11">
+        <f t="shared" si="0"/>
+        <v>8.1646560000000008</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="7">
+      <c r="I6" s="3">
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:9">
+      <c r="A7" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7" t="s">
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7" t="s">
+      <c r="F7" s="3"/>
+      <c r="G7" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="7"/>
+      <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="7" t="s">
+    <row r="8" spans="1:9">
+      <c r="A8" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7" t="s">
+      <c r="D8" s="3"/>
+      <c r="E8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7" t="s">
+      <c r="F8" s="3"/>
+      <c r="G8" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="7">
+      <c r="I8" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:9">
+      <c r="A9" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7" t="s">
+      <c r="D9" s="3"/>
+      <c r="E9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7" t="s">
+      <c r="F9" s="3"/>
+      <c r="G9" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="7"/>
+      <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="7" t="s">
+    <row r="10" spans="1:9">
+      <c r="A10" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="5">
         <v>39142</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="3">
         <v>2</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="3">
         <v>2900</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="11">
+        <f t="shared" si="0"/>
+        <v>1315.4168</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="7">
+      <c r="I10" s="3">
         <v>300</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="7" t="s">
+    <row r="11" spans="1:9">
+      <c r="A11" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="5">
         <v>37622</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="3">
         <v>1</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="3">
         <v>62</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="11">
+        <f t="shared" si="0"/>
+        <v>28.122703999999999</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="7">
+      <c r="I11" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="7" t="s">
+    <row r="12" spans="1:9">
+      <c r="A12" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="5">
         <v>38869</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="3">
         <v>3</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="3">
         <v>1000</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="11">
+        <f t="shared" si="0"/>
+        <v>453.59199999999998</v>
+      </c>
+      <c r="H12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="7">
+      <c r="I12" s="3">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="7" t="s">
+    <row r="13" spans="1:9">
+      <c r="A13" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7" t="s">
+      <c r="D13" s="3"/>
+      <c r="E13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7" t="s">
+      <c r="F13" s="3"/>
+      <c r="G13" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H13" s="7"/>
+      <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="7" t="s">
+    <row r="14" spans="1:9">
+      <c r="A14" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="3">
         <v>2</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="3">
         <v>30</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G14" s="11">
+        <f t="shared" si="0"/>
+        <v>13.607759999999999</v>
+      </c>
+      <c r="H14" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="H14" s="7">
+      <c r="I14" s="3">
         <v>0.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" s="5">
+        <v>41153</v>
+      </c>
+      <c r="D15" s="12">
+        <v>3</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="12">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G15" s="13">
+        <v>1</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15" s="12">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="C16" s="15">
+        <v>39965</v>
+      </c>
+      <c r="D16" s="12">
+        <v>2</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12">
+        <v>7.5</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16" s="12">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>